<commit_message>
Fix UI, Complete Data Permission
</commit_message>
<xml_diff>
--- a/assets/demo.xlsx
+++ b/assets/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elbechir/Sites/Front-Portal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91C45E8-FD6E-F249-BC5A-B67C290E353E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85F7A85-ED7F-8E49-AE55-AF388EE58B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,13 +88,13 @@
     <t>محمود</t>
   </si>
   <si>
-    <t xml:space="preserve">كتاب رقم 145 </t>
-  </si>
-  <si>
-    <t>كتاب رقم 146</t>
-  </si>
-  <si>
-    <t>كتاب رقم 147</t>
+    <t xml:space="preserve">كتاب رقم 245 </t>
+  </si>
+  <si>
+    <t>كتاب رقم 246</t>
+  </si>
+  <si>
+    <t>كتاب رقم 247</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>